<commit_message>
Create flow to bulk import lecturer list
</commit_message>
<xml_diff>
--- a/app/files/Part-Time Lecturer Requisition Form - template.xlsx
+++ b/app/files/Part-Time Lecturer Requisition Form - template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameliadavid/App/CourseXcel/app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E927885F-C12B-7A4D-950F-0FF35DCC0A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092DF98D-FE40-EE40-8987-70733D6C139A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-920" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Part-Time Lecturer Requisition Form</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Approved by HR</t>
+  </si>
+  <si>
+    <t>Name: Cheah Wan Theng</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
   <dimension ref="A3:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1438,7 @@
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="48" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="48" t="s">

</xml_diff>